<commit_message>
Site updated: 2020-07-03 19:53:58
</commit_message>
<xml_diff>
--- a/times/totaltime (1).xlsx
+++ b/times/totaltime (1).xlsx
@@ -11,7 +11,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
   <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;涓婂崍/涓嬪崍 &quot;hh&quot;鏅�&quot;mm&quot;鍒�&quot;ss&quot;绉� &quot;"/>
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -99,10 +99,10 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="锛汲 锛般偞銈枫儍銈�"/>
-        <a:font script="Hang" typeface="毵戩潃 瓿犽敃"/>
-        <a:font script="Hans" typeface="瀹嬩綋"/>
-        <a:font script="Hant" typeface="鏂扮窗鏄庨珨"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -134,10 +134,10 @@
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="锛汲 锛般偞銈枫儍銈�"/>
-        <a:font script="Hang" typeface="毵戩潃 瓿犽敃"/>
-        <a:font script="Hans" typeface="瀹嬩綋"/>
-        <a:font script="Hant" typeface="鏂扮窗鏄庨珨"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -393,13 +393,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B2" t="str">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C2" t="str">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>